<commit_message>
Upfate for python 2.7. Added csv directory
</commit_message>
<xml_diff>
--- a/SteinbergPrototype/WireMap.xlsx
+++ b/SteinbergPrototype/WireMap.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/t_mitcs/Documents/Catoptric/SteinbergPrototype/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC3DF0B9-71FC-B64E-99E1-BE74A3101F90}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4889454A-7326-FA48-9352-3DC6ED2BA37E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{02E2A21C-E7FC-0647-9A80-F89596A05ADF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
   <si>
     <t>Ground</t>
   </si>
@@ -58,6 +58,21 @@
   </si>
   <si>
     <t>Purple</t>
+  </si>
+  <si>
+    <t>Side of Box</t>
+  </si>
+  <si>
+    <t>Wire Color in Box</t>
+  </si>
+  <si>
+    <t>Wire Color between Mirrors</t>
+  </si>
+  <si>
+    <t>test setup</t>
+  </si>
+  <si>
+    <t>Grey</t>
   </si>
 </sst>
 </file>
@@ -409,136 +424,169 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCE590E7-ED3A-B246-9A62-06BD9669B12D}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="24.5" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1">
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D1">
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="F1">
+      <c r="F2">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="F2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3">
+      <c r="F3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>4</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
         <v>10</v>
       </c>
-      <c r="F5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E17" t="s">
-        <v>3</v>
-      </c>
-      <c r="F17">
+      <c r="F6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F20">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E21" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E22" t="s">
         <v>7</v>
       </c>
-      <c r="F21">
+      <c r="F22">
         <v>4</v>
       </c>
     </row>

</xml_diff>